<commit_message>
update column name: Vietnamese
</commit_message>
<xml_diff>
--- a/processed/combination_statistics.xlsx
+++ b/processed/combination_statistics.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Combination Statistics" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Thống kê tổ hợp" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -436,67 +436,67 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Year</t>
+          <t>Năm</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Region</t>
+          <t>Khu vực</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Province</t>
+          <t>Tỉnh/Thành phố</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Combination</t>
+          <t>Tổ hợp</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Number of Students</t>
+          <t>Số lượng thí sinh</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Average Score</t>
+          <t>Điểm trung bình</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Number of Scores &lt; 15</t>
+          <t>Số lượng điểm &lt; 15</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Number of Scores &lt; 20</t>
+          <t>Số lượng điểm &lt; 20</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Number of Scores &gt;= 27</t>
+          <t>Số lượng điểm &gt;= 27</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Max Score</t>
+          <t>Điểm cao nhất</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Min Score</t>
+          <t>Điểm thấp nhất</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Longitude</t>
+          <t>Kinh độ</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Latitude</t>
+          <t>Vĩ độ</t>
         </is>
       </c>
     </row>

</xml_diff>